<commit_message>
Ingresando al video 54 relacion uno a muchos
</commit_message>
<xml_diff>
--- a/Apuntes/Apuntes Curso Net Core.xlsx
+++ b/Apuntes/Apuntes Curso Net Core.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C05CFC-D2F5-43A1-940D-A0BC3514FF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>SECCION 4: Fundamentos de ASP.Net Core y Web API</t>
   </si>
@@ -109,12 +108,36 @@
   </si>
   <si>
     <t>Validaciones por atributo (Personalizadas)</t>
+  </si>
+  <si>
+    <t>DTOS y Autommer</t>
+  </si>
+  <si>
+    <t>Instalar autommaper.dependienci extension</t>
+  </si>
+  <si>
+    <t>Crear carpeta utilidades para guardar la clase de automapper</t>
+  </si>
+  <si>
+    <t>Instanciar automapper en el startup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear la clase de autommaper </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   CreateMap&lt;AutorCreacionDTO, Autor&gt;();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ctrl + r + r </t>
+  </si>
+  <si>
+    <t>Renombra variables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,14 +169,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,42 +456,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="6" width="16.77734375" customWidth="1"/>
+    <col min="2" max="6" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="L2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
       <c r="L3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="L4" t="s">
         <v>20</v>
       </c>
@@ -476,86 +499,86 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>14</v>
       </c>
@@ -563,7 +586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>16</v>
       </c>
@@ -571,23 +594,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="K27" t="s">
+        <v>32</v>
+      </c>
+      <c r="L27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
@@ -596,17 +625,43 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="1" t="s">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E40" s="4"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>